<commit_message>
Complete functionality of kivy app
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -40,6 +40,9 @@
     <t>Operating profit</t>
   </si>
   <si>
+    <t>2019-12-3</t>
+  </si>
+  <si>
     <t>2015-12-3</t>
   </si>
   <si>
@@ -49,12 +52,12 @@
     <t>2016-12-3</t>
   </si>
   <si>
-    <t>2019-12-3</t>
-  </si>
-  <si>
     <t>2017-12-3</t>
   </si>
   <si>
+    <t>115585000</t>
+  </si>
+  <si>
     <t>118779000</t>
   </si>
   <si>
@@ -64,34 +67,31 @@
     <t>105590000</t>
   </si>
   <si>
-    <t>115585000</t>
-  </si>
-  <si>
     <t>112269000</t>
   </si>
   <si>
+    <t>0.067</t>
+  </si>
+  <si>
     <t>0.028</t>
   </si>
   <si>
     <t>0.032</t>
   </si>
   <si>
-    <t>0.067</t>
-  </si>
-  <si>
     <t>4560000</t>
   </si>
   <si>
+    <t>3701000</t>
+  </si>
+  <si>
+    <t>8822000</t>
+  </si>
+  <si>
+    <t>3136000</t>
+  </si>
+  <si>
     <t>6140000</t>
-  </si>
-  <si>
-    <t>3701000</t>
-  </si>
-  <si>
-    <t>8822000</t>
-  </si>
-  <si>
-    <t>3136000</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -599,10 +599,10 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -616,10 +616,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -633,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
@@ -653,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -667,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -718,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
@@ -752,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>

</xml_diff>